<commit_message>
changes to presentation - costs
</commit_message>
<xml_diff>
--- a/Engineering/2018-2019/Project Field Safety/Costs.xlsx
+++ b/Engineering/2018-2019/Project Field Safety/Costs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/silasjohnson/Documents/GitHub/UNHSEDS/Engineering/2018-2019/Project Field Safety/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5277C4-0973-FD44-B6F2-C4A3CD899740}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B37E92-893D-7A4F-9372-78B83CB3ECA4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="24860" windowHeight="13440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -475,7 +475,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>